<commit_message>
Move SAND to prod
</commit_message>
<xml_diff>
--- a/Projects/INBEVTRADMX/Data/inbevtradmx_template.xlsx
+++ b/Projects/INBEVTRADMX/Data/inbevtradmx_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="1" state="visible" r:id="rId2"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="149">
   <si>
     <t xml:space="preserve">KPI Level 1 Name</t>
   </si>
@@ -128,24 +128,7 @@
     <t xml:space="preserve">POS</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">"Nothing to Tag", "Uniforme", "Corcholata Entrada", "Logo Modelorama Exterior", "Termometro", </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">2X58 1X33 MEGA CORONA LIGHT, Mega light, Premium Stella Michelob Cucapa_Sabor para conocedores, TendCardTriptico_Michelob, TendCardTriptico_Stella Artois, TendCardTriptico_Cucapa, 1X30MEGAC, 1X28MEGAC, Michelob POS Other, Stella Artois POS Other, Cucapa POS Other</t>
-    </r>
+    <t xml:space="preserve">"Nothing to Tag", "Uniforme", "Corcholata Entrada", "Logo Modelorama Exterior", "Termometro"</t>
   </si>
   <si>
     <t xml:space="preserve">N/A</t>
@@ -214,9 +197,6 @@
     <t xml:space="preserve">POP Agua</t>
   </si>
   <si>
-    <t xml:space="preserve">"Nothing to Tag", "Uniforme", "Corcholata Entrada", "Logo Modelorama Exterior", "Termometro"</t>
-  </si>
-  <si>
     <t xml:space="preserve">Nestle, Nestle - Santa Maria, SANTA MARIA</t>
   </si>
   <si>
@@ -379,7 +359,7 @@
     <t xml:space="preserve">Invasión</t>
   </si>
   <si>
-    <t xml:space="preserve">Cerveza, COOLERS, CRAFT &amp; IMPORTS, ENERGIZANTE, LIGHT, PREMIUM, REGULAR, REGULAR/CLARA, REGULAR/OBSCURA, SIN ALCOHOL, VALUE , Other</t>
+    <t xml:space="preserve">Cerveza, COOLERS, CRAFT &amp; IMPORTS, ENERGIZANTE, LIGHT, PREMIUM, REGULAR, REGULAR/CLARA, REGULAR/OBSCURA, SIN ALCOHOL, VALUE</t>
   </si>
   <si>
     <t xml:space="preserve">Purity KPI: Pass if only product type: SKU, OTHER or EMPTY are found in the cooler for selected manufacturers and category. 100% purity target.</t>
@@ -424,9 +404,6 @@
     <t xml:space="preserve">Pepsi</t>
   </si>
   <si>
-    <t xml:space="preserve">SKU, Other, Empty, Irrelevant</t>
-  </si>
-  <si>
     <t xml:space="preserve">Product Availability KPI: If in scene type "Cooler" there is at least 1 facing for Manufacturer: "Pepsi" for Product Type: SKU, then pass.</t>
   </si>
   <si>
@@ -457,7 +434,10 @@
     <t xml:space="preserve">Sabritas Vacío</t>
   </si>
   <si>
-    <t xml:space="preserve">100% of Share must be Product Type SKU or Other. No empty spaces are allowed.</t>
+    <t xml:space="preserve">100% of Share must be Product Type SKU or Other from category "Botana". No empty spaces are allowed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_type, store_type, template_name,category</t>
   </si>
   <si>
     <t xml:space="preserve">Purity KPI: Pass if only product type: SKU, OTHER or EMPTY are found in the scene type "Sabritas" for selected manufacturer "Sabritas" 100% purity target.</t>
@@ -533,7 +513,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -569,18 +549,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -673,7 +641,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -698,10 +666,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -718,7 +682,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -730,11 +694,11 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -818,36 +782,35 @@
   <dimension ref="A1:T39"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="18" topLeftCell="L19" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="18" topLeftCell="S19" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="L1" activeCellId="0" sqref="L1"/>
+      <selection pane="topRight" activeCell="S1" activeCellId="0" sqref="S1"/>
       <selection pane="bottomLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
-      <selection pane="bottomRight" activeCell="M19" activeCellId="0" sqref="M19"/>
+      <selection pane="bottomRight" activeCell="D21" activeCellId="0" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="58.4489795918367"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="58.5867346938776"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="49"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="30.1020408163265"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="99.3520408163265"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="27.5408163265306"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="26.3214285714286"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="33.6122448979592"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="99.3520408163265"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="106.510204081633"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="59.8010204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="59.9387755102041"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="50.0816326530612"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="30.780612244898"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="101.515306122449"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="28.0765306122449"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="27.1326530612245"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="34.4234693877551"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="101.515306122449"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="108.938775510204"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -925,7 +888,7 @@
       <c r="D2" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="0" t="s">
         <v>23</v>
       </c>
       <c r="F2" s="0" t="s">
@@ -964,7 +927,7 @@
       <c r="Q2" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="R2" s="7" t="s">
+      <c r="R2" s="6" t="s">
         <v>29</v>
       </c>
       <c r="S2" s="0" t="s">
@@ -1011,7 +974,7 @@
       <c r="Q3" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="R3" s="7" t="s">
+      <c r="R3" s="6" t="s">
         <v>36</v>
       </c>
       <c r="S3" s="0" t="s">
@@ -1064,7 +1027,7 @@
       <c r="Q4" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="R4" s="7" t="s">
+      <c r="R4" s="6" t="s">
         <v>42</v>
       </c>
       <c r="S4" s="0" t="s">
@@ -1088,7 +1051,7 @@
         <v>22</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>46</v>
+        <v>23</v>
       </c>
       <c r="H5" s="0" t="s">
         <v>24</v>
@@ -1100,7 +1063,7 @@
         <v>24</v>
       </c>
       <c r="M5" s="0" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N5" s="0" t="n">
         <v>5</v>
@@ -1114,11 +1077,11 @@
       <c r="Q5" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="R5" s="8" t="s">
+      <c r="R5" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="S5" s="0" t="s">
         <v>48</v>
-      </c>
-      <c r="S5" s="0" t="s">
-        <v>49</v>
       </c>
       <c r="T5" s="0" t="s">
         <v>31</v>
@@ -1128,14 +1091,14 @@
       <c r="A6" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" s="0" t="s">
         <v>50</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>51</v>
       </c>
       <c r="H6" s="0" t="s">
         <v>24</v>
@@ -1144,7 +1107,7 @@
         <v>25</v>
       </c>
       <c r="L6" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M6" s="0" t="s">
         <v>24</v>
@@ -1161,13 +1124,13 @@
       <c r="Q6" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="R6" s="8" t="s">
+      <c r="R6" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S6" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="S6" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="T6" s="10" t="s">
+      <c r="T6" s="9" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1176,10 +1139,10 @@
         <v>20</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D7" s="0" t="s">
         <v>24</v>
@@ -1188,10 +1151,10 @@
         <v>3</v>
       </c>
       <c r="H7" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="I7" s="0" t="s">
         <v>56</v>
-      </c>
-      <c r="I7" s="0" t="s">
-        <v>57</v>
       </c>
       <c r="J7" s="0" t="s">
         <v>24</v>
@@ -1214,13 +1177,13 @@
       <c r="Q7" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="R7" s="7" t="s">
-        <v>58</v>
+      <c r="R7" s="6" t="s">
+        <v>57</v>
       </c>
       <c r="S7" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="T7" s="10" t="s">
+      <c r="T7" s="9" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1229,13 +1192,13 @@
         <v>20</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H8" s="0" t="s">
         <v>24</v>
@@ -1244,7 +1207,7 @@
         <v>25</v>
       </c>
       <c r="L8" s="0" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="M8" s="0" t="s">
         <v>24</v>
@@ -1261,13 +1224,13 @@
       <c r="Q8" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="R8" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="S8" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="T8" s="10" t="s">
+      <c r="R8" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="S8" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="T8" s="9" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1276,13 +1239,13 @@
         <v>20</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H9" s="0" t="s">
         <v>24</v>
@@ -1291,7 +1254,7 @@
         <v>25</v>
       </c>
       <c r="L9" s="0" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="M9" s="0" t="s">
         <v>24</v>
@@ -1308,13 +1271,13 @@
       <c r="Q9" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="R9" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="S9" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="T9" s="10" t="s">
+      <c r="R9" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="S9" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="T9" s="9" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1323,13 +1286,13 @@
         <v>20</v>
       </c>
       <c r="B10" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" s="0" t="s">
         <v>65</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>66</v>
       </c>
       <c r="H10" s="0" t="s">
         <v>24</v>
@@ -1355,69 +1318,69 @@
       <c r="Q10" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="R10" s="8" t="s">
+      <c r="R10" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="S10" s="10" t="s">
         <v>67</v>
-      </c>
-      <c r="S10" s="11" t="s">
-        <v>68</v>
       </c>
       <c r="T10" s="0" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="11" s="9" customFormat="true" ht="14" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="9" t="s">
+    <row r="11" s="8" customFormat="true" ht="14" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D11" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="C11" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="D11" s="9" t="s">
+      <c r="F11" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="F11" s="12" t="s">
+      <c r="H11" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="J11" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="L11" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="M11" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="N11" s="8" t="n">
+        <v>10</v>
+      </c>
+      <c r="O11" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="P11" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q11" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="R11" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="H11" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="J11" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="L11" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="M11" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="N11" s="9" t="n">
-        <v>10</v>
-      </c>
-      <c r="O11" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="P11" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q11" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="R11" s="13" t="s">
+      <c r="S11" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="S11" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="T11" s="9" t="s">
+      <c r="T11" s="8" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>21</v>
@@ -1429,7 +1392,7 @@
         <v>22</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>46</v>
+        <v>23</v>
       </c>
       <c r="H12" s="0" t="s">
         <v>24</v>
@@ -1450,12 +1413,12 @@
         <v>26</v>
       </c>
       <c r="P12" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q12" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="Q12" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="R12" s="7" t="s">
+      <c r="R12" s="6" t="s">
         <v>29</v>
       </c>
       <c r="S12" s="0" t="s">
@@ -1467,7 +1430,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B13" s="0" t="s">
         <v>32</v>
@@ -1482,7 +1445,7 @@
         <v>24</v>
       </c>
       <c r="J13" s="0" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="L13" s="0" t="s">
         <v>24</v>
@@ -1497,12 +1460,12 @@
         <v>26</v>
       </c>
       <c r="P13" s="0" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="Q13" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="R13" s="7" t="s">
+      <c r="R13" s="6" t="s">
         <v>36</v>
       </c>
       <c r="S13" s="0" t="s">
@@ -1514,13 +1477,13 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D14" s="0" t="s">
         <v>24</v>
@@ -1529,10 +1492,10 @@
         <v>5</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J14" s="0" t="s">
         <v>24</v>
@@ -1550,13 +1513,13 @@
         <v>26</v>
       </c>
       <c r="P14" s="0" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="Q14" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="R14" s="7" t="s">
-        <v>80</v>
+      <c r="R14" s="6" t="s">
+        <v>79</v>
       </c>
       <c r="S14" s="0" t="s">
         <v>43</v>
@@ -1567,13 +1530,13 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D15" s="0" t="s">
         <v>24</v>
@@ -1582,10 +1545,10 @@
         <v>8</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J15" s="0" t="s">
         <v>24</v>
@@ -1603,13 +1566,13 @@
         <v>26</v>
       </c>
       <c r="P15" s="0" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="Q15" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="R15" s="7" t="s">
-        <v>83</v>
+      <c r="R15" s="6" t="s">
+        <v>82</v>
       </c>
       <c r="S15" s="0" t="s">
         <v>43</v>
@@ -1620,16 +1583,16 @@
     </row>
     <row r="16" customFormat="false" ht="14" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H16" s="0" t="s">
         <v>24</v>
@@ -1638,7 +1601,7 @@
         <v>25</v>
       </c>
       <c r="L16" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M16" s="0" t="s">
         <v>24</v>
@@ -1650,30 +1613,30 @@
         <v>26</v>
       </c>
       <c r="P16" s="0" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="Q16" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="R16" s="8" t="s">
+      <c r="R16" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S16" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="S16" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="T16" s="10" t="s">
+      <c r="T16" s="9" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D17" s="0" t="s">
         <v>24</v>
@@ -1682,10 +1645,10 @@
         <v>7</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I17" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J17" s="0" t="s">
         <v>24</v>
@@ -1703,13 +1666,13 @@
         <v>26</v>
       </c>
       <c r="P17" s="0" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="Q17" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="R17" s="7" t="s">
-        <v>87</v>
+      <c r="R17" s="6" t="s">
+        <v>86</v>
       </c>
       <c r="S17" s="0" t="s">
         <v>43</v>
@@ -1720,16 +1683,16 @@
     </row>
     <row r="18" customFormat="false" ht="14" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H18" s="0" t="s">
         <v>24</v>
@@ -1750,16 +1713,16 @@
         <v>26</v>
       </c>
       <c r="P18" s="0" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="Q18" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="R18" s="8" t="s">
+      <c r="R18" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="S18" s="10" t="s">
         <v>67</v>
-      </c>
-      <c r="S18" s="11" t="s">
-        <v>68</v>
       </c>
       <c r="T18" s="0" t="s">
         <v>38</v>
@@ -1767,17 +1730,17 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="B19" s="0" t="s">
         <v>89</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="C19" s="0" t="s">
         <v>90</v>
       </c>
-      <c r="C19" s="0" t="s">
+      <c r="D19" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="D19" s="0" t="s">
-        <v>92</v>
-      </c>
       <c r="G19" s="0" t="s">
         <v>24</v>
       </c>
@@ -1788,7 +1751,7 @@
         <v>24</v>
       </c>
       <c r="K19" s="0" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L19" s="0" t="s">
         <v>24</v>
@@ -1800,19 +1763,19 @@
         <v>10</v>
       </c>
       <c r="O19" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="P19" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q19" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="R19" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="P19" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q19" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="R19" s="8" t="s">
+      <c r="S19" s="0" t="s">
         <v>94</v>
-      </c>
-      <c r="S19" s="0" t="s">
-        <v>95</v>
       </c>
       <c r="T19" s="0" t="s">
         <v>31</v>
@@ -1820,16 +1783,16 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B20" s="0" t="s">
         <v>35</v>
       </c>
       <c r="C20" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="D20" s="0" t="s">
         <v>96</v>
-      </c>
-      <c r="D20" s="0" t="s">
-        <v>97</v>
       </c>
       <c r="G20" s="0" t="s">
         <v>24</v>
@@ -1853,7 +1816,7 @@
         <v>2</v>
       </c>
       <c r="O20" s="0" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="P20" s="0" t="s">
         <v>24</v>
@@ -1861,11 +1824,11 @@
       <c r="Q20" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="R20" s="8" t="s">
+      <c r="R20" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="S20" s="10" t="s">
         <v>98</v>
-      </c>
-      <c r="S20" s="11" t="s">
-        <v>99</v>
       </c>
       <c r="T20" s="0" t="s">
         <v>38</v>
@@ -1873,13 +1836,13 @@
     </row>
     <row r="21" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B21" s="0" t="s">
         <v>35</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D21" s="0" t="s">
         <v>33</v>
@@ -1894,7 +1857,7 @@
         <v>25</v>
       </c>
       <c r="K21" s="0" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L21" s="0" t="s">
         <v>24</v>
@@ -1906,7 +1869,7 @@
         <v>2</v>
       </c>
       <c r="O21" s="0" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="P21" s="0" t="s">
         <v>24</v>
@@ -1914,11 +1877,11 @@
       <c r="Q21" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="R21" s="8" t="s">
+      <c r="R21" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="S21" s="14" t="s">
         <v>102</v>
-      </c>
-      <c r="S21" s="15" t="s">
-        <v>103</v>
       </c>
       <c r="T21" s="0" t="s">
         <v>38</v>
@@ -1926,16 +1889,16 @@
     </row>
     <row r="22" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B22" s="0" t="s">
         <v>35</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G22" s="0" t="s">
         <v>24</v>
@@ -1959,7 +1922,7 @@
         <v>6</v>
       </c>
       <c r="O22" s="0" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="P22" s="0" t="s">
         <v>24</v>
@@ -1967,11 +1930,11 @@
       <c r="Q22" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="R22" s="8" t="s">
+      <c r="R22" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="S22" s="0" t="s">
         <v>105</v>
-      </c>
-      <c r="S22" s="0" t="s">
-        <v>106</v>
       </c>
       <c r="T22" s="0" t="s">
         <v>31</v>
@@ -1979,16 +1942,16 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C23" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="D23" s="0" t="s">
         <v>96</v>
-      </c>
-      <c r="D23" s="0" t="s">
-        <v>97</v>
       </c>
       <c r="G23" s="0" t="s">
         <v>24</v>
@@ -2012,19 +1975,19 @@
         <v>2</v>
       </c>
       <c r="O23" s="0" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="P23" s="0" t="s">
         <v>24</v>
       </c>
       <c r="Q23" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="R23" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="R23" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="S23" s="11" t="s">
-        <v>99</v>
+      <c r="S23" s="10" t="s">
+        <v>98</v>
       </c>
       <c r="T23" s="0" t="s">
         <v>38</v>
@@ -2032,13 +1995,13 @@
     </row>
     <row r="24" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D24" s="0" t="s">
         <v>33</v>
@@ -2050,7 +2013,7 @@
         <v>24</v>
       </c>
       <c r="J24" s="0" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K24" s="0" t="s">
         <v>24</v>
@@ -2065,19 +2028,19 @@
         <v>2</v>
       </c>
       <c r="O24" s="0" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="P24" s="0" t="s">
         <v>24</v>
       </c>
       <c r="Q24" s="0" t="s">
-        <v>108</v>
-      </c>
-      <c r="R24" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="S24" s="15" t="s">
-        <v>106</v>
+        <v>107</v>
+      </c>
+      <c r="R24" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="S24" s="14" t="s">
+        <v>105</v>
       </c>
       <c r="T24" s="0" t="s">
         <v>38</v>
@@ -2085,16 +2048,16 @@
     </row>
     <row r="25" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G25" s="0" t="s">
         <v>24</v>
@@ -2103,7 +2066,7 @@
         <v>24</v>
       </c>
       <c r="J25" s="0" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K25" s="0" t="s">
         <v>24</v>
@@ -2118,19 +2081,19 @@
         <v>6</v>
       </c>
       <c r="O25" s="0" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="P25" s="0" t="s">
         <v>24</v>
       </c>
       <c r="Q25" s="0" t="s">
-        <v>108</v>
-      </c>
-      <c r="R25" s="8" t="s">
-        <v>112</v>
+        <v>107</v>
+      </c>
+      <c r="R25" s="7" t="s">
+        <v>111</v>
       </c>
       <c r="S25" s="0" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="T25" s="0" t="s">
         <v>31</v>
@@ -2138,16 +2101,16 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C26" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="D26" s="0" t="s">
         <v>96</v>
-      </c>
-      <c r="D26" s="0" t="s">
-        <v>97</v>
       </c>
       <c r="G26" s="0" t="s">
         <v>24</v>
@@ -2171,33 +2134,33 @@
         <v>2</v>
       </c>
       <c r="O26" s="0" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="P26" s="0" t="s">
         <v>24</v>
       </c>
       <c r="Q26" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="R26" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="R26" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="S26" s="11" t="s">
-        <v>99</v>
+      <c r="S26" s="10" t="s">
+        <v>98</v>
       </c>
       <c r="T26" s="0" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D27" s="0" t="s">
         <v>33</v>
@@ -2209,7 +2172,7 @@
         <v>24</v>
       </c>
       <c r="J27" s="0" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K27" s="0" t="s">
         <v>24</v>
@@ -2224,19 +2187,19 @@
         <v>2</v>
       </c>
       <c r="O27" s="0" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="P27" s="0" t="s">
         <v>24</v>
       </c>
       <c r="Q27" s="0" t="s">
-        <v>113</v>
-      </c>
-      <c r="R27" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="S27" s="15" t="s">
-        <v>106</v>
+        <v>112</v>
+      </c>
+      <c r="R27" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="S27" s="14" t="s">
+        <v>105</v>
       </c>
       <c r="T27" s="0" t="s">
         <v>38</v>
@@ -2244,16 +2207,16 @@
     </row>
     <row r="28" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="G28" s="0" t="s">
         <v>24</v>
@@ -2262,7 +2225,7 @@
         <v>24</v>
       </c>
       <c r="J28" s="0" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K28" s="0" t="s">
         <v>24</v>
@@ -2277,19 +2240,19 @@
         <v>6</v>
       </c>
       <c r="O28" s="0" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="P28" s="0" t="s">
         <v>24</v>
       </c>
       <c r="Q28" s="0" t="s">
-        <v>113</v>
-      </c>
-      <c r="R28" s="8" t="s">
-        <v>117</v>
+        <v>112</v>
+      </c>
+      <c r="R28" s="7" t="s">
+        <v>115</v>
       </c>
       <c r="S28" s="0" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="T28" s="0" t="s">
         <v>31</v>
@@ -2297,16 +2260,16 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G29" s="0" t="s">
         <v>24</v>
@@ -2324,19 +2287,19 @@
         <v>2</v>
       </c>
       <c r="O29" s="0" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="P29" s="0" t="s">
         <v>24</v>
       </c>
       <c r="Q29" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="R29" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="R29" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="S29" s="11" t="s">
-        <v>99</v>
+      <c r="S29" s="10" t="s">
+        <v>98</v>
       </c>
       <c r="T29" s="0" t="s">
         <v>38</v>
@@ -2344,13 +2307,13 @@
     </row>
     <row r="30" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D30" s="0" t="s">
         <v>33</v>
@@ -2362,10 +2325,10 @@
         <v>24</v>
       </c>
       <c r="J30" s="0" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="K30" s="0" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="L30" s="0" t="s">
         <v>24</v>
@@ -2377,19 +2340,19 @@
         <v>2</v>
       </c>
       <c r="O30" s="0" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="P30" s="0" t="s">
         <v>24</v>
       </c>
       <c r="Q30" s="0" t="s">
-        <v>118</v>
-      </c>
-      <c r="R30" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="S30" s="15" t="s">
-        <v>103</v>
+        <v>116</v>
+      </c>
+      <c r="R30" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="S30" s="14" t="s">
+        <v>102</v>
       </c>
       <c r="T30" s="0" t="s">
         <v>38</v>
@@ -2397,16 +2360,16 @@
     </row>
     <row r="31" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G31" s="0" t="s">
         <v>24</v>
@@ -2415,10 +2378,10 @@
         <v>24</v>
       </c>
       <c r="J31" s="0" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="K31" s="0" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="L31" s="0" t="s">
         <v>24</v>
@@ -2430,19 +2393,19 @@
         <v>6</v>
       </c>
       <c r="O31" s="0" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="P31" s="0" t="s">
         <v>24</v>
       </c>
       <c r="Q31" s="0" t="s">
-        <v>118</v>
-      </c>
-      <c r="R31" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="S31" s="15" t="s">
-        <v>103</v>
+        <v>116</v>
+      </c>
+      <c r="R31" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="S31" s="14" t="s">
+        <v>102</v>
       </c>
       <c r="T31" s="0" t="s">
         <v>31</v>
@@ -2450,22 +2413,25 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G32" s="0" t="s">
         <v>24</v>
       </c>
       <c r="H32" s="0" t="s">
         <v>24</v>
+      </c>
+      <c r="K32" s="0" t="s">
+        <v>120</v>
       </c>
       <c r="L32" s="0" t="s">
         <v>24</v>
@@ -2477,19 +2443,19 @@
         <v>1</v>
       </c>
       <c r="O32" s="0" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="P32" s="0" t="s">
         <v>24</v>
       </c>
       <c r="Q32" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="R32" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="R32" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="S32" s="11" t="s">
-        <v>99</v>
+      <c r="S32" s="10" t="s">
+        <v>126</v>
       </c>
       <c r="T32" s="0" t="s">
         <v>38</v>
@@ -2497,13 +2463,13 @@
     </row>
     <row r="33" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D33" s="0" t="s">
         <v>33</v>
@@ -2515,28 +2481,28 @@
         <v>24</v>
       </c>
       <c r="J33" s="0" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="K33" s="0" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="N33" s="0" t="n">
         <v>1</v>
       </c>
       <c r="O33" s="0" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="P33" s="0" t="s">
         <v>24</v>
       </c>
       <c r="Q33" s="0" t="s">
-        <v>125</v>
-      </c>
-      <c r="R33" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="S33" s="15" t="s">
-        <v>103</v>
+        <v>123</v>
+      </c>
+      <c r="R33" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="S33" s="14" t="s">
+        <v>102</v>
       </c>
       <c r="T33" s="0" t="s">
         <v>38</v>
@@ -2544,16 +2510,16 @@
     </row>
     <row r="34" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G34" s="0" t="s">
         <v>24</v>
@@ -2562,28 +2528,28 @@
         <v>24</v>
       </c>
       <c r="J34" s="0" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="K34" s="0" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="N34" s="0" t="n">
         <v>3</v>
       </c>
       <c r="O34" s="0" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="P34" s="0" t="s">
         <v>24</v>
       </c>
       <c r="Q34" s="0" t="s">
-        <v>125</v>
-      </c>
-      <c r="R34" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="S34" s="15" t="s">
-        <v>103</v>
+        <v>123</v>
+      </c>
+      <c r="R34" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="S34" s="14" t="s">
+        <v>102</v>
       </c>
       <c r="T34" s="0" t="s">
         <v>31</v>
@@ -2591,13 +2557,13 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B35" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="C35" s="0" t="s">
         <v>130</v>
-      </c>
-      <c r="C35" s="0" t="s">
-        <v>131</v>
       </c>
       <c r="D35" s="0" t="s">
         <v>22</v>
@@ -2624,19 +2590,19 @@
         <v>10</v>
       </c>
       <c r="O35" s="0" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="P35" s="0" t="s">
         <v>24</v>
       </c>
       <c r="Q35" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="R35" s="0" t="s">
         <v>132</v>
       </c>
-      <c r="R35" s="0" t="s">
-        <v>133</v>
-      </c>
-      <c r="S35" s="11" t="s">
-        <v>99</v>
+      <c r="S35" s="10" t="s">
+        <v>98</v>
       </c>
       <c r="T35" s="0" t="s">
         <v>31</v>
@@ -2644,13 +2610,13 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B36" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="C36" s="0" t="s">
         <v>134</v>
-      </c>
-      <c r="C36" s="0" t="s">
-        <v>135</v>
       </c>
       <c r="D36" s="0" t="s">
         <v>22</v>
@@ -2677,19 +2643,19 @@
         <v>10</v>
       </c>
       <c r="O36" s="0" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="P36" s="0" t="s">
         <v>24</v>
       </c>
       <c r="Q36" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="R36" s="0" t="s">
         <v>136</v>
       </c>
-      <c r="R36" s="0" t="s">
-        <v>137</v>
-      </c>
-      <c r="S36" s="11" t="s">
-        <v>99</v>
+      <c r="S36" s="10" t="s">
+        <v>98</v>
       </c>
       <c r="T36" s="0" t="s">
         <v>31</v>
@@ -2697,13 +2663,13 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D37" s="0" t="s">
         <v>22</v>
@@ -2730,19 +2696,19 @@
         <v>10</v>
       </c>
       <c r="O37" s="0" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="P37" s="0" t="s">
         <v>24</v>
       </c>
       <c r="Q37" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="R37" s="0" t="s">
         <v>139</v>
       </c>
-      <c r="R37" s="0" t="s">
-        <v>140</v>
-      </c>
-      <c r="S37" s="11" t="s">
-        <v>99</v>
+      <c r="S37" s="10" t="s">
+        <v>98</v>
       </c>
       <c r="T37" s="0" t="s">
         <v>31</v>
@@ -2750,19 +2716,19 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B38" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="C38" s="0" t="s">
         <v>141</v>
-      </c>
-      <c r="C38" s="0" t="s">
-        <v>142</v>
       </c>
       <c r="D38" s="0" t="s">
         <v>22</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G38" s="0" t="s">
         <v>24</v>
@@ -2786,19 +2752,19 @@
         <v>10</v>
       </c>
       <c r="O38" s="0" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="P38" s="0" t="s">
         <v>24</v>
       </c>
       <c r="Q38" s="0" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="R38" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="S38" s="10" t="s">
         <v>144</v>
-      </c>
-      <c r="S38" s="11" t="s">
-        <v>145</v>
       </c>
       <c r="T38" s="0" t="s">
         <v>31</v>
@@ -2806,19 +2772,19 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B39" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="C39" s="0" t="s">
         <v>146</v>
-      </c>
-      <c r="C39" s="0" t="s">
-        <v>147</v>
       </c>
       <c r="D39" s="0" t="s">
         <v>22</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G39" s="0" t="s">
         <v>24</v>
@@ -2842,19 +2808,19 @@
         <v>5</v>
       </c>
       <c r="O39" s="0" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="P39" s="0" t="s">
         <v>24</v>
       </c>
       <c r="Q39" s="0" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="R39" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="S39" s="11" t="s">
-        <v>145</v>
+        <v>147</v>
+      </c>
+      <c r="S39" s="10" t="s">
+        <v>144</v>
       </c>
       <c r="T39" s="0" t="s">
         <v>31</v>
@@ -2884,20 +2850,23 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="10" t="s">
-        <v>149</v>
+      <c r="A1" s="9" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="9" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="10" t="s">
-        <v>93</v>
+      <c r="A3" s="9" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>